<commit_message>
change µC to STM32H573
</commit_message>
<xml_diff>
--- a/docs/IO_Funktion_Beschreibung.xlsx
+++ b/docs/IO_Funktion_Beschreibung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proj\RoboticLawnMower\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5CF0DABE-442B-4307-86D6-463399FDEADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF947F1C-1AA4-47CF-9C78-CB7413AADFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
   <si>
     <t>Bezeichnung</t>
   </si>
@@ -138,9 +138,6 @@
     <t>Sensor</t>
   </si>
   <si>
-    <t>Systemstrom</t>
-  </si>
-  <si>
     <t>Kompass</t>
   </si>
   <si>
@@ -189,24 +186,9 @@
     <t>Schleifen-Sensor</t>
   </si>
   <si>
-    <t>???</t>
-  </si>
-  <si>
-    <t>RegenSensor</t>
-  </si>
-  <si>
     <t>Komfort</t>
   </si>
   <si>
-    <t>GSM</t>
-  </si>
-  <si>
-    <t>USART 2</t>
-  </si>
-  <si>
-    <t>GSM Modul</t>
-  </si>
-  <si>
     <t>ESP32</t>
   </si>
   <si>
@@ -216,12 +198,6 @@
     <t>WLAN/BT Kommunikation (Evtl. Kamera)</t>
   </si>
   <si>
-    <t>I/O's</t>
-  </si>
-  <si>
-    <t>I/O' zwischen ESP und AVR</t>
-  </si>
-  <si>
     <t>WS2128</t>
   </si>
   <si>
@@ -240,9 +216,6 @@
     <t>Bremslicht</t>
   </si>
   <si>
-    <t>Blinklicht</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -255,9 +228,6 @@
     <t>Höhenverstellung Mähwerk</t>
   </si>
   <si>
-    <t>GPIO/SPI/ADC</t>
-  </si>
-  <si>
     <t>FRAM</t>
   </si>
   <si>
@@ -270,14 +240,41 @@
     <t>?</t>
   </si>
   <si>
-    <t>GPIO/ADC</t>
+    <t>GPIO - OpenDrain</t>
+  </si>
+  <si>
+    <t>GPIO PWR EN</t>
+  </si>
+  <si>
+    <t>STM32H573</t>
+  </si>
+  <si>
+    <t>I2C - 3</t>
+  </si>
+  <si>
+    <t>GPS EN</t>
+  </si>
+  <si>
+    <t>Sig</t>
+  </si>
+  <si>
+    <t>Counter</t>
+  </si>
+  <si>
+    <t>Input Counter</t>
+  </si>
+  <si>
+    <t>CTR</t>
+  </si>
+  <si>
+    <t>TIM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,8 +322,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +353,11 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -368,12 +377,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -406,9 +416,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -417,9 +424,17 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Schlecht" xfId="2" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -434,6 +449,191 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>382635</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>172540</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27951532-470E-9D04-D2E4-770092C738E6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7439025" y="152400"/>
+          <a:ext cx="10031460" cy="6687640"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>49531</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rechteck 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{934D8C1F-6DA9-C20B-805D-E9C9084C4B63}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13782675" y="1383031"/>
+          <a:ext cx="1419225" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>87631</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rechteck 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F35C4FC2-927E-4F11-AC48-A669D394BB89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13458825" y="3897631"/>
+          <a:ext cx="1419225" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFC000"/>
+        </a:solidFill>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:srgbClr val="FF0000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -699,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="X19" sqref="X19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -710,9 +910,10 @@
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -727,16 +928,16 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="12"/>
+      <c r="B2" s="16"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
         <v>5</v>
@@ -750,17 +951,17 @@
       <c r="E3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F3" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="D4" s="6">
         <v>3</v>
@@ -768,15 +969,11 @@
       <c r="E4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="13">
-        <v>3</v>
-      </c>
-      <c r="H4" s="13"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F4" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="5" t="s">
         <v>10</v>
@@ -790,8 +987,11 @@
       <c r="E5" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F5" s="14" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -800,7 +1000,7 @@
       <c r="D6" s="3"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="5" t="s">
         <v>14</v>
@@ -814,21 +1014,21 @@
       <c r="E7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="13"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="5" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="13"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F8" s="12"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="7" t="s">
         <v>19</v>
@@ -837,609 +1037,788 @@
         <v>6</v>
       </c>
       <c r="D9" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F9" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="7" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="D10" s="8">
         <v>1</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D11" s="8">
         <v>1</v>
       </c>
       <c r="E11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="12"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="13"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="5" t="s">
+      <c r="F12" s="12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="5" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="13"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="8">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="13"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="F13" s="12"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>6</v>
       </c>
       <c r="D14" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="13"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="7" t="s">
-        <v>23</v>
+        <v>76</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
+      <c r="B16" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16" s="8">
+        <v>1</v>
+      </c>
       <c r="E16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="13"/>
+        <v>22</v>
+      </c>
+      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="7" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D17" s="8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="13"/>
+        <v>25</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D18" s="8">
-        <v>1</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F18" s="13"/>
+      <c r="B18" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="18"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D19" s="8">
-        <v>1</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="D19" s="8"/>
       <c r="E19" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F19" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="5" t="s">
-        <v>30</v>
+      <c r="B20" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
       <c r="E20" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F20" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D21" s="6">
+      <c r="D21" s="8">
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="13"/>
+        <v>22</v>
+      </c>
+      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="5" t="s">
-        <v>30</v>
+      <c r="B22" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
       <c r="E22" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="F22" s="13"/>
+        <v>25</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="6">
-        <v>1</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F23" s="13"/>
+      <c r="B23" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="12"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="5" t="s">
-        <v>30</v>
+      <c r="B24" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D24" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="D24" s="8"/>
       <c r="E24" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="F24" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="7" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="6">
+        <v>77</v>
+      </c>
+      <c r="D25" s="8">
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F25" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="7" t="s">
-        <v>67</v>
+        <v>21</v>
       </c>
       <c r="C26" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26" s="8">
         <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="F26" s="13"/>
+        <v>22</v>
+      </c>
+      <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="7" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="6">
-        <v>1</v>
+        <v>24</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F27" s="13"/>
+        <v>25</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="4"/>
+      <c r="A28" s="1"/>
+      <c r="B28" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="12"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="5" t="s">
-        <v>45</v>
+      <c r="B29" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D29" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
       <c r="E29" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="13"/>
+        <v>20</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="5" t="s">
-        <v>70</v>
+      <c r="B30" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D30" s="1"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="13"/>
+        <v>77</v>
+      </c>
+      <c r="D30" s="8">
+        <v>1</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="5" t="s">
-        <v>71</v>
+      <c r="B31" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D31" s="1"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="13"/>
+        <v>6</v>
+      </c>
+      <c r="D31" s="8">
+        <v>1</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F31" s="12"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="5" t="s">
-        <v>30</v>
+      <c r="B32" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D32" s="1"/>
+        <v>24</v>
+      </c>
+      <c r="D32" s="8">
+        <v>0</v>
+      </c>
       <c r="E32" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F32" s="16"/>
+        <v>25</v>
+      </c>
+      <c r="F32" s="12" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="7" t="s">
-        <v>32</v>
+      <c r="B33" s="5" t="s">
+        <v>30</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D33" s="6">
-        <v>1</v>
-      </c>
+        <v>15</v>
+      </c>
+      <c r="D33" s="1"/>
       <c r="E33" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F33" s="16"/>
+        <v>31</v>
+      </c>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="5" t="s">
-        <v>38</v>
+      <c r="B34" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>39</v>
+        <v>6</v>
       </c>
       <c r="D34" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F34" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="5" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="F35" s="13"/>
+        <v>34</v>
+      </c>
+      <c r="F35" s="12"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="5" t="s">
-        <v>43</v>
+      <c r="B36" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D36" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="D36" s="6"/>
       <c r="E36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="F36" s="12"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="5" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F37" s="13"/>
+        <v>35</v>
+      </c>
+      <c r="F37" s="12"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="5" t="s">
-        <v>47</v>
+      <c r="B38" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="D38" s="6">
+        <v>1</v>
+      </c>
       <c r="E38" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F38" s="13"/>
+        <v>33</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="5" t="s">
-        <v>49</v>
+      <c r="B39" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>50</v>
+        <v>6</v>
       </c>
       <c r="D39" s="6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F39" s="16"/>
+        <v>60</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="5" t="s">
-        <v>52</v>
+      <c r="B40" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D40" s="6">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F40" s="16"/>
+        <v>61</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="6">
+      <c r="A41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D42" s="6">
         <v>1</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="4"/>
+      <c r="E42" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F42" s="12"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="5" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>58</v>
+        <v>14</v>
       </c>
       <c r="D43" s="6">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>59</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="F43" s="12"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="5" t="s">
-        <v>60</v>
+        <v>37</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>61</v>
+        <v>38</v>
       </c>
       <c r="D44" s="6">
         <v>2</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>62</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="F44" s="12"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
-      <c r="B45" s="7" t="s">
-        <v>63</v>
+      <c r="B45" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="6">
-        <v>4</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D45" s="1"/>
       <c r="E45" s="5" t="s">
-        <v>64</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="F45" s="12"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
-      <c r="B46" s="7" t="s">
-        <v>72</v>
+      <c r="B46" s="5" t="s">
+        <v>42</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D46" s="6"/>
-      <c r="E46" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F46" s="12"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
-      <c r="B47" s="7" t="s">
-        <v>73</v>
+      <c r="B47" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D47" s="6"/>
-      <c r="E47" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="D47" s="6">
+        <v>2</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F47" s="12"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
+      <c r="D48" s="1"/>
       <c r="E48" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F48" s="12"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D49" s="6">
+        <v>2</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F49" s="15"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
-      <c r="B49" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="C49" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D49" s="6"/>
-      <c r="E49" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="9"/>
-      <c r="B50" s="10" t="s">
+      <c r="F50" s="15"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D51" s="6">
+        <v>3</v>
+      </c>
+      <c r="E51" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F51" s="15"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="1"/>
+      <c r="F52" s="12"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="3"/>
+      <c r="E53" s="4"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="1"/>
+      <c r="B54" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D54" s="6">
+        <v>5</v>
+      </c>
+      <c r="E54" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="1"/>
+      <c r="B55" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="5"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="1"/>
+      <c r="B56" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="5"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="1"/>
+      <c r="B57" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="C50" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="D50" s="11">
-        <v>2</v>
-      </c>
-      <c r="E50" s="10" t="s">
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="6">
-        <v>42</v>
-      </c>
-      <c r="E51" s="1"/>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1"/>
+      <c r="B58" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D58" s="6">
+        <v>4</v>
+      </c>
+      <c r="E58" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="C59" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="11"/>
+      <c r="E59" s="10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="1"/>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1"/>
+      <c r="D60" s="6">
+        <f>SUM(D3:D59)</f>
+        <v>44</v>
+      </c>
+      <c r="E60" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62">
+        <v>49</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1447,5 +1826,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>